<commit_message>
allow to edit existing configurations
</commit_message>
<xml_diff>
--- a/documents/time-records/Lorenz-Oberhammer.xlsx
+++ b/documents/time-records/Lorenz-Oberhammer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24123"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QE\Documents\Work\Nabu\03_Teaching\02_Courses\Software Engineering\SS21\Templates - Projektabwicklung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC9B9862-AE6E-4451-90EE-716A8A1279D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4835849E-8C0D-49B1-99CE-2410BCF3829D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28425" yWindow="4020" windowWidth="28245" windowHeight="17565" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="46">
   <si>
     <t>Datum</t>
   </si>
@@ -156,13 +156,25 @@
     <t>Issue Nr. 68</t>
   </si>
   <si>
+    <t>Issues Nr. 71, 83, 86</t>
+  </si>
+  <si>
+    <t>Docker Lösung testen mit Würfel</t>
+  </si>
+  <si>
+    <t>Systemtest (fremdes System)</t>
+  </si>
+  <si>
+    <t>Installation fremdes System</t>
+  </si>
+  <si>
+    <t>Issue Nr. 129</t>
+  </si>
+  <si>
     <t>ID</t>
   </si>
   <si>
     <t>Bezeichnung</t>
-  </si>
-  <si>
-    <t>Systemtest (fremdes System)</t>
   </si>
   <si>
     <t>Abschlussbericht</t>
@@ -580,11 +592,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F855F84B-A166-7442-8B83-EBB2C6A67214}">
-  <dimension ref="A1:D1016"/>
+  <dimension ref="A1:D1017"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B58" sqref="B58"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C51" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="B72" sqref="B72"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
@@ -1394,69 +1406,178 @@
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="8"/>
-      <c r="B59" s="7"/>
+      <c r="A59" s="8">
+        <v>44326</v>
+      </c>
+      <c r="B59" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C59" t="s">
+        <v>4</v>
+      </c>
       <c r="D59" s="3"/>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="8"/>
-      <c r="B60" s="7"/>
-      <c r="D60" s="3"/>
+      <c r="A60" s="8">
+        <v>44327</v>
+      </c>
+      <c r="B60" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C60" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="8"/>
-      <c r="B61" s="7"/>
-      <c r="D61" s="3"/>
+      <c r="A61" s="8">
+        <v>44328</v>
+      </c>
+      <c r="B61" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C61" t="s">
+        <v>21</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="8"/>
-      <c r="B62" s="7"/>
-      <c r="D62" s="3"/>
+      <c r="A62" s="8">
+        <v>44328</v>
+      </c>
+      <c r="B62" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C62" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="8"/>
-      <c r="B63" s="7"/>
-      <c r="D63" s="3"/>
+      <c r="A63" s="8">
+        <v>44329</v>
+      </c>
+      <c r="B63" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C63" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="8"/>
-      <c r="B64" s="7"/>
-      <c r="D64" s="3"/>
+      <c r="A64" s="8">
+        <v>44329</v>
+      </c>
+      <c r="B64" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C64" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="8"/>
-      <c r="B65" s="7"/>
-      <c r="D65" s="3"/>
+      <c r="A65" s="8">
+        <v>44333</v>
+      </c>
+      <c r="B65" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C65" t="s">
+        <v>38</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="8"/>
-      <c r="B66" s="7"/>
+      <c r="A66" s="8">
+        <v>44333</v>
+      </c>
+      <c r="B66" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C66" t="s">
+        <v>38</v>
+      </c>
       <c r="D66" s="3"/>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="8"/>
-      <c r="B67" s="7"/>
+      <c r="A67" s="8">
+        <v>44335</v>
+      </c>
+      <c r="B67" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C67" t="s">
+        <v>38</v>
+      </c>
       <c r="D67" s="3"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="8"/>
-      <c r="B68" s="7"/>
-      <c r="D68" s="3"/>
+      <c r="A68" s="8">
+        <v>44335</v>
+      </c>
+      <c r="B68" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C68" t="s">
+        <v>38</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="8"/>
-      <c r="B69" s="7"/>
+      <c r="A69" s="8">
+        <v>44336</v>
+      </c>
+      <c r="B69" s="7">
+        <v>0.125</v>
+      </c>
+      <c r="C69" t="s">
+        <v>38</v>
+      </c>
       <c r="D69" s="3"/>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="8"/>
-      <c r="B70" s="7"/>
-      <c r="D70" s="3"/>
+      <c r="A70" s="8">
+        <v>44343</v>
+      </c>
+      <c r="B70" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C70" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="8"/>
-      <c r="B71" s="7"/>
-      <c r="D71" s="3"/>
+      <c r="A71" s="8">
+        <v>44345</v>
+      </c>
+      <c r="B71" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C71" t="s">
+        <v>21</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="8"/>
@@ -6179,7 +6300,12 @@
       <c r="D1015" s="3"/>
     </row>
     <row r="1016" spans="1:4">
-      <c r="A1016" s="2"/>
+      <c r="A1016" s="8"/>
+      <c r="B1016" s="7"/>
+      <c r="D1016" s="3"/>
+    </row>
+    <row r="1017" spans="1:4">
+      <c r="A1017" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -6191,7 +6317,7 @@
           <x14:formula1>
             <xm:f>Tätigkeiten!$B$2:$B$12</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1015</xm:sqref>
+          <xm:sqref>C2:C1016</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6212,10 +6338,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6247,7 +6373,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6255,7 +6381,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6287,7 +6413,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2">

</xml_diff>